<commit_message>
added corsconfig for githubpages
</commit_message>
<xml_diff>
--- a/src/main/resources/transaksjoner.xlsx
+++ b/src/main/resources/transaksjoner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bjorn\Prosjekter\stacc\SavingApp -backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B1EF29-57C4-421C-93C6-619357495849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9658BD15-43DF-44C5-A58D-BA129A798BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,9 +469,6 @@
     <t>25.07.2023</t>
   </si>
   <si>
-    <t>Nettgiro fra: Bjørn Hagen Betalt: 25.07.23</t>
-  </si>
-  <si>
     <t>REDD BARNA Betalt: 25.07.23</t>
   </si>
   <si>
@@ -1505,6 +1502,9 @@
   </si>
   <si>
     <t>ferie</t>
+  </si>
+  <si>
+    <t>Nettgiro fra: fdgdfgg Betalt: 25.07.23</t>
   </si>
 </sst>
 </file>
@@ -1890,8 +1890,8 @@
   <sheetPr codeName="Transaksjoner"/>
   <dimension ref="A1:F235"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="C178" sqref="C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1904,27 +1904,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" t="s">
         <v>237</v>
       </c>
-      <c r="B1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>235</v>
       </c>
-      <c r="D1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E1" t="s">
-        <v>236</v>
-      </c>
       <c r="F1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -1939,12 +1939,12 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -1959,18 +1959,18 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D4">
         <v>-3775</v>
@@ -1979,18 +1979,18 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5">
         <v>1000</v>
@@ -1999,18 +1999,18 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D6">
         <v>-1000</v>
@@ -2019,18 +2019,18 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B7" t="s">
         <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D7">
         <v>-4000</v>
@@ -2039,12 +2039,12 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B8" t="s">
         <v>123</v>
@@ -2059,18 +2059,18 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B9" t="s">
         <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D9">
         <v>-300</v>
@@ -2079,12 +2079,12 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B10" t="s">
         <v>123</v>
@@ -2099,18 +2099,18 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C11" t="s">
         <v>226</v>
-      </c>
-      <c r="C11" t="s">
-        <v>227</v>
       </c>
       <c r="D11">
         <v>-270</v>
@@ -2119,18 +2119,18 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B12" t="s">
+        <v>225</v>
+      </c>
+      <c r="C12" t="s">
         <v>226</v>
-      </c>
-      <c r="C12" t="s">
-        <v>227</v>
       </c>
       <c r="D12">
         <v>-270</v>
@@ -2139,18 +2139,18 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D13">
         <v>-174.7</v>
@@ -2159,18 +2159,18 @@
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D14">
         <v>-372.9</v>
@@ -2179,18 +2179,18 @@
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D15">
         <v>-95</v>
@@ -2199,18 +2199,18 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D16">
         <v>-95</v>
@@ -2219,18 +2219,18 @@
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D17">
         <v>-37</v>
@@ -2239,12 +2239,12 @@
         <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B18" t="s">
         <v>118</v>
@@ -2259,12 +2259,12 @@
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B19" t="s">
         <v>118</v>
@@ -2279,12 +2279,12 @@
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B20" t="s">
         <v>118</v>
@@ -2299,12 +2299,12 @@
         <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B21" t="s">
         <v>118</v>
@@ -2319,18 +2319,18 @@
         <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B22" t="s">
+        <v>222</v>
+      </c>
+      <c r="C22" t="s">
         <v>223</v>
-      </c>
-      <c r="C22" t="s">
-        <v>224</v>
       </c>
       <c r="D22">
         <v>-50</v>
@@ -2339,18 +2339,18 @@
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D23">
         <v>-39</v>
@@ -2359,12 +2359,12 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B24" t="s">
         <v>114</v>
@@ -2379,12 +2379,12 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B25" t="s">
         <v>114</v>
@@ -2399,12 +2399,12 @@
         <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B26" t="s">
         <v>114</v>
@@ -2419,12 +2419,12 @@
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -2439,12 +2439,12 @@
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B28" t="s">
         <v>10</v>
@@ -2459,18 +2459,18 @@
         <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D29">
         <v>-10.9</v>
@@ -2479,12 +2479,12 @@
         <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -2499,12 +2499,12 @@
         <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
@@ -2519,18 +2519,18 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B32" t="s">
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D32">
         <v>-95</v>
@@ -2539,12 +2539,12 @@
         <v>2</v>
       </c>
       <c r="F32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B33" t="s">
         <v>10</v>
@@ -2559,12 +2559,12 @@
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -2579,18 +2579,18 @@
         <v>2</v>
       </c>
       <c r="F34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B35" t="s">
+        <v>217</v>
+      </c>
+      <c r="C35" t="s">
         <v>218</v>
-      </c>
-      <c r="C35" t="s">
-        <v>219</v>
       </c>
       <c r="D35">
         <v>-99</v>
@@ -2599,18 +2599,18 @@
         <v>2</v>
       </c>
       <c r="F35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B36" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D36">
         <v>-117.3</v>
@@ -2619,18 +2619,18 @@
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D37">
         <v>-189</v>
@@ -2639,18 +2639,18 @@
         <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B38" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C38" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D38">
         <v>-58</v>
@@ -2659,18 +2659,18 @@
         <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B39" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C39" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D39">
         <v>-65</v>
@@ -2679,12 +2679,12 @@
         <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
@@ -2699,18 +2699,18 @@
         <v>2</v>
       </c>
       <c r="F40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D41">
         <v>-917</v>
@@ -2719,12 +2719,12 @@
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B42" t="s">
         <v>5</v>
@@ -2739,12 +2739,12 @@
         <v>2</v>
       </c>
       <c r="F42" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
@@ -2759,12 +2759,12 @@
         <v>2</v>
       </c>
       <c r="F43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B44" t="s">
         <v>5</v>
@@ -2779,18 +2779,18 @@
         <v>2</v>
       </c>
       <c r="F44" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B45" t="s">
+        <v>215</v>
+      </c>
+      <c r="C45" t="s">
         <v>216</v>
-      </c>
-      <c r="C45" t="s">
-        <v>217</v>
       </c>
       <c r="D45">
         <v>-21.9</v>
@@ -2799,12 +2799,12 @@
         <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B46" t="s">
         <v>0</v>
@@ -2819,12 +2819,12 @@
         <v>2</v>
       </c>
       <c r="F46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B47" t="s">
         <v>0</v>
@@ -2839,12 +2839,12 @@
         <v>2</v>
       </c>
       <c r="F47" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B48" t="s">
         <v>0</v>
@@ -2859,18 +2859,18 @@
         <v>2</v>
       </c>
       <c r="F48" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B49" t="s">
+        <v>211</v>
+      </c>
+      <c r="C49" t="s">
         <v>212</v>
-      </c>
-      <c r="C49" t="s">
-        <v>213</v>
       </c>
       <c r="D49">
         <v>-278.39999999999998</v>
@@ -2879,18 +2879,18 @@
         <v>2</v>
       </c>
       <c r="F49" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B50" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D50">
         <v>-275.81</v>
@@ -2899,18 +2899,18 @@
         <v>2</v>
       </c>
       <c r="F50" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C51" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D51">
         <v>-40</v>
@@ -2919,12 +2919,12 @@
         <v>2</v>
       </c>
       <c r="F51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B52" t="s">
         <v>107</v>
@@ -2939,12 +2939,12 @@
         <v>2</v>
       </c>
       <c r="F52" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B53" t="s">
         <v>107</v>
@@ -2959,12 +2959,12 @@
         <v>2</v>
       </c>
       <c r="F53" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B54" t="s">
         <v>107</v>
@@ -2979,12 +2979,12 @@
         <v>2</v>
       </c>
       <c r="F54" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B55" t="s">
         <v>107</v>
@@ -2999,12 +2999,12 @@
         <v>2</v>
       </c>
       <c r="F55" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B56" t="s">
         <v>107</v>
@@ -3019,12 +3019,12 @@
         <v>2</v>
       </c>
       <c r="F56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B57" t="s">
         <v>107</v>
@@ -3039,18 +3039,18 @@
         <v>2</v>
       </c>
       <c r="F57" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B58" t="s">
         <v>107</v>
       </c>
       <c r="C58" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D58">
         <v>1000</v>
@@ -3059,18 +3059,18 @@
         <v>2</v>
       </c>
       <c r="F58" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B59" t="s">
         <v>107</v>
       </c>
       <c r="C59" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D59">
         <v>-1000</v>
@@ -3079,12 +3079,12 @@
         <v>2</v>
       </c>
       <c r="F59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B60" t="s">
         <v>100</v>
@@ -3099,12 +3099,12 @@
         <v>2</v>
       </c>
       <c r="F60" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B61" t="s">
         <v>100</v>
@@ -3119,12 +3119,12 @@
         <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B62" t="s">
         <v>100</v>
@@ -3139,12 +3139,12 @@
         <v>2</v>
       </c>
       <c r="F62" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B63" t="s">
         <v>100</v>
@@ -3159,12 +3159,12 @@
         <v>2</v>
       </c>
       <c r="F63" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B64" t="s">
         <v>100</v>
@@ -3179,18 +3179,18 @@
         <v>2</v>
       </c>
       <c r="F64" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B65" t="s">
         <v>100</v>
       </c>
       <c r="C65" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D65">
         <v>210</v>
@@ -3199,12 +3199,12 @@
         <v>2</v>
       </c>
       <c r="F65" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B66" t="s">
         <v>100</v>
@@ -3219,18 +3219,18 @@
         <v>2</v>
       </c>
       <c r="F66" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B67" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C67" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D67">
         <v>1000</v>
@@ -3239,18 +3239,18 @@
         <v>2</v>
       </c>
       <c r="F67" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B68" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C68" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D68">
         <v>-1000</v>
@@ -3259,12 +3259,12 @@
         <v>2</v>
       </c>
       <c r="F68" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B69" t="s">
         <v>98</v>
@@ -3279,18 +3279,18 @@
         <v>2</v>
       </c>
       <c r="F69" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B70" t="s">
+        <v>198</v>
+      </c>
+      <c r="C70" t="s">
         <v>199</v>
-      </c>
-      <c r="C70" t="s">
-        <v>200</v>
       </c>
       <c r="D70">
         <v>-160</v>
@@ -3299,18 +3299,18 @@
         <v>2</v>
       </c>
       <c r="F70" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C71" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D71">
         <v>-33</v>
@@ -3319,18 +3319,18 @@
         <v>2</v>
       </c>
       <c r="F71" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B72" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C72" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D72">
         <v>-131</v>
@@ -3339,18 +3339,18 @@
         <v>2</v>
       </c>
       <c r="F72" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B73" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C73" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D73">
         <v>-25</v>
@@ -3359,18 +3359,18 @@
         <v>2</v>
       </c>
       <c r="F73" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C74" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D74">
         <v>-40</v>
@@ -3379,18 +3379,18 @@
         <v>2</v>
       </c>
       <c r="F74" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B75" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C75" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D75">
         <v>-303.5</v>
@@ -3399,18 +3399,18 @@
         <v>2</v>
       </c>
       <c r="F75" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B76" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C76" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D76">
         <v>-155</v>
@@ -3419,18 +3419,18 @@
         <v>2</v>
       </c>
       <c r="F76" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B77" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C77" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D77">
         <v>-100</v>
@@ -3439,18 +3439,18 @@
         <v>2</v>
       </c>
       <c r="F77" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B78" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C78" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D78">
         <v>-69</v>
@@ -3459,18 +3459,18 @@
         <v>2</v>
       </c>
       <c r="F78" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B79" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C79" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D79">
         <v>-97.3</v>
@@ -3479,18 +3479,18 @@
         <v>2</v>
       </c>
       <c r="F79" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B80" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C80" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D80">
         <v>-105</v>
@@ -3499,18 +3499,18 @@
         <v>2</v>
       </c>
       <c r="F80" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B81" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C81" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D81">
         <v>-89</v>
@@ -3519,18 +3519,18 @@
         <v>2</v>
       </c>
       <c r="F81" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B82" t="s">
+        <v>196</v>
+      </c>
+      <c r="C82" t="s">
         <v>197</v>
-      </c>
-      <c r="C82" t="s">
-        <v>198</v>
       </c>
       <c r="D82">
         <v>-270</v>
@@ -3539,18 +3539,18 @@
         <v>2</v>
       </c>
       <c r="F82" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B83" t="s">
+        <v>196</v>
+      </c>
+      <c r="C83" t="s">
         <v>197</v>
-      </c>
-      <c r="C83" t="s">
-        <v>198</v>
       </c>
       <c r="D83">
         <v>-270</v>
@@ -3559,12 +3559,12 @@
         <v>2</v>
       </c>
       <c r="F83" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B84" t="s">
         <v>94</v>
@@ -3579,12 +3579,12 @@
         <v>2</v>
       </c>
       <c r="F84" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B85" t="s">
         <v>94</v>
@@ -3599,12 +3599,12 @@
         <v>2</v>
       </c>
       <c r="F85" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B86" t="s">
         <v>94</v>
@@ -3619,18 +3619,18 @@
         <v>2</v>
       </c>
       <c r="F86" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B87" t="s">
         <v>94</v>
       </c>
       <c r="C87" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D87">
         <v>1000</v>
@@ -3639,18 +3639,18 @@
         <v>2</v>
       </c>
       <c r="F87" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B88" t="s">
+        <v>193</v>
+      </c>
+      <c r="C88" t="s">
         <v>194</v>
-      </c>
-      <c r="C88" t="s">
-        <v>195</v>
       </c>
       <c r="D88">
         <v>-194.9</v>
@@ -3659,18 +3659,18 @@
         <v>2</v>
       </c>
       <c r="F88" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B89" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C89" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D89">
         <v>-449.12</v>
@@ -3679,18 +3679,18 @@
         <v>2</v>
       </c>
       <c r="F89" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B90" t="s">
+        <v>188</v>
+      </c>
+      <c r="C90" t="s">
         <v>189</v>
-      </c>
-      <c r="C90" t="s">
-        <v>190</v>
       </c>
       <c r="D90">
         <v>-160</v>
@@ -3699,18 +3699,18 @@
         <v>2</v>
       </c>
       <c r="F90" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B91" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C91" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D91">
         <v>-518</v>
@@ -3719,18 +3719,18 @@
         <v>2</v>
       </c>
       <c r="F91" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B92" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C92" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D92">
         <v>-23</v>
@@ -3739,18 +3739,18 @@
         <v>2</v>
       </c>
       <c r="F92" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B93" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C93" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D93">
         <v>-51.82</v>
@@ -3759,18 +3759,18 @@
         <v>2</v>
       </c>
       <c r="F93" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B94" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C94" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D94">
         <v>-2549</v>
@@ -3779,18 +3779,18 @@
         <v>2</v>
       </c>
       <c r="F94" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B95" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C95" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D95">
         <v>1000</v>
@@ -3799,18 +3799,18 @@
         <v>2</v>
       </c>
       <c r="F95" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B96" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C96" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D96">
         <v>-1000</v>
@@ -3819,18 +3819,18 @@
         <v>2</v>
       </c>
       <c r="F96" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B97" t="s">
+        <v>182</v>
+      </c>
+      <c r="C97" t="s">
         <v>183</v>
-      </c>
-      <c r="C97" t="s">
-        <v>184</v>
       </c>
       <c r="D97">
         <v>-87.8</v>
@@ -3839,18 +3839,18 @@
         <v>2</v>
       </c>
       <c r="F97" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B98" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C98" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D98">
         <v>-115</v>
@@ -3859,18 +3859,18 @@
         <v>2</v>
       </c>
       <c r="F98" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B99" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C99" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D99">
         <v>-61.11</v>
@@ -3879,18 +3879,18 @@
         <v>2</v>
       </c>
       <c r="F99" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B100" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C100" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D100">
         <v>-220</v>
@@ -3899,18 +3899,18 @@
         <v>2</v>
       </c>
       <c r="F100" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B101" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C101" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D101">
         <v>-592.22</v>
@@ -3919,18 +3919,18 @@
         <v>2</v>
       </c>
       <c r="F101" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B102" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C102" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D102">
         <v>-23</v>
@@ -3939,18 +3939,18 @@
         <v>2</v>
       </c>
       <c r="F102" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B103" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C103" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D103">
         <v>-370.58</v>
@@ -3959,12 +3959,12 @@
         <v>2</v>
       </c>
       <c r="F103" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B104" t="s">
         <v>90</v>
@@ -3979,12 +3979,12 @@
         <v>2</v>
       </c>
       <c r="F104" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B105" t="s">
         <v>90</v>
@@ -3999,12 +3999,12 @@
         <v>2</v>
       </c>
       <c r="F105" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B106" t="s">
         <v>90</v>
@@ -4019,12 +4019,12 @@
         <v>2</v>
       </c>
       <c r="F106" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B107" t="s">
         <v>88</v>
@@ -4039,18 +4039,18 @@
         <v>2</v>
       </c>
       <c r="F107" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B108" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C108" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D108">
         <v>1000</v>
@@ -4059,18 +4059,18 @@
         <v>2</v>
       </c>
       <c r="F108" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B109" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C109" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D109">
         <v>-1000</v>
@@ -4079,12 +4079,12 @@
         <v>2</v>
       </c>
       <c r="F109" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B110" t="s">
         <v>86</v>
@@ -4099,18 +4099,18 @@
         <v>2</v>
       </c>
       <c r="F110" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B111" t="s">
+        <v>167</v>
+      </c>
+      <c r="C111" t="s">
         <v>168</v>
-      </c>
-      <c r="C111" t="s">
-        <v>169</v>
       </c>
       <c r="D111">
         <v>-102.66</v>
@@ -4119,18 +4119,18 @@
         <v>2</v>
       </c>
       <c r="F111" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B112" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C112" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D112">
         <v>-10.06</v>
@@ -4139,18 +4139,18 @@
         <v>2</v>
       </c>
       <c r="F112" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B113" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C113" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D113">
         <v>-36</v>
@@ -4159,18 +4159,18 @@
         <v>2</v>
       </c>
       <c r="F113" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B114" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C114" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D114">
         <v>-424.74</v>
@@ -4179,18 +4179,18 @@
         <v>2</v>
       </c>
       <c r="F114" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B115" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C115" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D115">
         <v>-431.17</v>
@@ -4199,18 +4199,18 @@
         <v>2</v>
       </c>
       <c r="F115" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B116" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C116" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D116">
         <v>-109.2</v>
@@ -4219,18 +4219,18 @@
         <v>2</v>
       </c>
       <c r="F116" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B117" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C117" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D117">
         <v>-36</v>
@@ -4239,18 +4239,18 @@
         <v>2</v>
       </c>
       <c r="F117" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B118" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C118" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D118">
         <v>-26.17</v>
@@ -4259,18 +4259,18 @@
         <v>2</v>
       </c>
       <c r="F118" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B119" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C119" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D119">
         <v>-40.26</v>
@@ -4279,18 +4279,18 @@
         <v>2</v>
       </c>
       <c r="F119" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B120" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C120" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D120">
         <v>-258.67</v>
@@ -4299,18 +4299,18 @@
         <v>2</v>
       </c>
       <c r="F120" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B121" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C121" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D121">
         <v>-1000</v>
@@ -4319,18 +4319,18 @@
         <v>2</v>
       </c>
       <c r="F121" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B122" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C122" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D122">
         <v>-2158.2199999999998</v>
@@ -4339,18 +4339,18 @@
         <v>2</v>
       </c>
       <c r="F122" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B123" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C123" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D123">
         <v>-32.21</v>
@@ -4359,18 +4359,18 @@
         <v>2</v>
       </c>
       <c r="F123" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B124" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C124" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D124">
         <v>-398</v>
@@ -4379,18 +4379,18 @@
         <v>2</v>
       </c>
       <c r="F124" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B125" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C125" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D125">
         <v>-56.38</v>
@@ -4399,18 +4399,18 @@
         <v>2</v>
       </c>
       <c r="F125" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B126" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C126" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D126">
         <v>-4800</v>
@@ -4419,12 +4419,12 @@
         <v>2</v>
       </c>
       <c r="F126" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B127" t="s">
         <v>81</v>
@@ -4439,12 +4439,12 @@
         <v>2</v>
       </c>
       <c r="F127" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B128" t="s">
         <v>81</v>
@@ -4459,12 +4459,12 @@
         <v>2</v>
       </c>
       <c r="F128" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B129" t="s">
         <v>81</v>
@@ -4479,12 +4479,12 @@
         <v>2</v>
       </c>
       <c r="F129" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B130" t="s">
         <v>81</v>
@@ -4499,18 +4499,18 @@
         <v>2</v>
       </c>
       <c r="F130" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B131" t="s">
         <v>81</v>
       </c>
       <c r="C131" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D131">
         <v>500</v>
@@ -4519,18 +4519,18 @@
         <v>2</v>
       </c>
       <c r="F131" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B132" t="s">
+        <v>163</v>
+      </c>
+      <c r="C132" t="s">
         <v>164</v>
-      </c>
-      <c r="C132" t="s">
-        <v>165</v>
       </c>
       <c r="D132">
         <v>-22.49</v>
@@ -4539,18 +4539,18 @@
         <v>2</v>
       </c>
       <c r="F132" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B133" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C133" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D133">
         <v>-239.54</v>
@@ -4559,18 +4559,18 @@
         <v>2</v>
       </c>
       <c r="F133" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B134" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C134" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D134">
         <v>-600.87</v>
@@ -4579,12 +4579,12 @@
         <v>2</v>
       </c>
       <c r="F134" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B135" t="s">
         <v>79</v>
@@ -4599,18 +4599,18 @@
         <v>2</v>
       </c>
       <c r="F135" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B136" t="s">
+        <v>159</v>
+      </c>
+      <c r="C136" t="s">
         <v>160</v>
-      </c>
-      <c r="C136" t="s">
-        <v>161</v>
       </c>
       <c r="D136">
         <v>-131.44</v>
@@ -4619,18 +4619,18 @@
         <v>2</v>
       </c>
       <c r="F136" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B137" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C137" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D137">
         <v>-82.61</v>
@@ -4639,18 +4639,18 @@
         <v>2</v>
       </c>
       <c r="F137" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B138" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C138" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D138">
         <v>-137.53</v>
@@ -4659,18 +4659,18 @@
         <v>2</v>
       </c>
       <c r="F138" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B139" t="s">
+        <v>156</v>
+      </c>
+      <c r="C139" t="s">
         <v>157</v>
-      </c>
-      <c r="C139" t="s">
-        <v>158</v>
       </c>
       <c r="D139">
         <v>-146.31</v>
@@ -4679,18 +4679,18 @@
         <v>2</v>
       </c>
       <c r="F139" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B140" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C140" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D140">
         <v>-6000</v>
@@ -4699,18 +4699,18 @@
         <v>2</v>
       </c>
       <c r="F140" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B141" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C141" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D141">
         <v>1000</v>
@@ -4719,18 +4719,18 @@
         <v>2</v>
       </c>
       <c r="F141" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B142" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C142" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D142">
         <v>-1000</v>
@@ -4739,18 +4739,18 @@
         <v>2</v>
       </c>
       <c r="F142" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B143" t="s">
+        <v>154</v>
+      </c>
+      <c r="C143" t="s">
         <v>155</v>
-      </c>
-      <c r="C143" t="s">
-        <v>156</v>
       </c>
       <c r="D143">
         <v>-236</v>
@@ -4759,12 +4759,12 @@
         <v>2</v>
       </c>
       <c r="F143" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B144" t="s">
         <v>68</v>
@@ -4779,12 +4779,12 @@
         <v>2</v>
       </c>
       <c r="F144" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B145" t="s">
         <v>68</v>
@@ -4799,12 +4799,12 @@
         <v>2</v>
       </c>
       <c r="F145" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B146" t="s">
         <v>68</v>
@@ -4819,12 +4819,12 @@
         <v>2</v>
       </c>
       <c r="F146" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B147" t="s">
         <v>68</v>
@@ -4839,12 +4839,12 @@
         <v>2</v>
       </c>
       <c r="F147" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B148" t="s">
         <v>68</v>
@@ -4859,12 +4859,12 @@
         <v>2</v>
       </c>
       <c r="F148" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B149" t="s">
         <v>68</v>
@@ -4879,12 +4879,12 @@
         <v>2</v>
       </c>
       <c r="F149" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B150" t="s">
         <v>68</v>
@@ -4899,12 +4899,12 @@
         <v>2</v>
       </c>
       <c r="F150" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B151" t="s">
         <v>68</v>
@@ -4919,12 +4919,12 @@
         <v>2</v>
       </c>
       <c r="F151" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B152" t="s">
         <v>68</v>
@@ -4939,12 +4939,12 @@
         <v>2</v>
       </c>
       <c r="F152" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B153" t="s">
         <v>68</v>
@@ -4959,12 +4959,12 @@
         <v>2</v>
       </c>
       <c r="F153" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B154" t="s">
         <v>64</v>
@@ -4979,12 +4979,12 @@
         <v>2</v>
       </c>
       <c r="F154" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B155" t="s">
         <v>64</v>
@@ -4999,12 +4999,12 @@
         <v>2</v>
       </c>
       <c r="F155" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B156" t="s">
         <v>64</v>
@@ -5019,18 +5019,18 @@
         <v>2</v>
       </c>
       <c r="F156" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B157" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C157" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D157">
         <v>1000</v>
@@ -5039,18 +5039,18 @@
         <v>2</v>
       </c>
       <c r="F157" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B158" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C158" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D158">
         <v>-1000</v>
@@ -5059,18 +5059,18 @@
         <v>2</v>
       </c>
       <c r="F158" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B159" t="s">
         <v>59</v>
       </c>
       <c r="C159" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D159">
         <v>556</v>
@@ -5079,12 +5079,12 @@
         <v>2</v>
       </c>
       <c r="F159" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B160" t="s">
         <v>59</v>
@@ -5099,12 +5099,12 @@
         <v>2</v>
       </c>
       <c r="F160" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B161" t="s">
         <v>59</v>
@@ -5119,12 +5119,12 @@
         <v>2</v>
       </c>
       <c r="F161" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B162" t="s">
         <v>59</v>
@@ -5139,12 +5139,12 @@
         <v>2</v>
       </c>
       <c r="F162" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B163" t="s">
         <v>59</v>
@@ -5159,18 +5159,18 @@
         <v>2</v>
       </c>
       <c r="F163" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B164" t="s">
+        <v>150</v>
+      </c>
+      <c r="C164" t="s">
         <v>151</v>
-      </c>
-      <c r="C164" t="s">
-        <v>152</v>
       </c>
       <c r="D164">
         <v>-53</v>
@@ -5179,18 +5179,18 @@
         <v>2</v>
       </c>
       <c r="F164" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B165" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C165" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D165">
         <v>-112.48</v>
@@ -5199,18 +5199,18 @@
         <v>2</v>
       </c>
       <c r="F165" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B166" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C166" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D166">
         <v>-99</v>
@@ -5219,12 +5219,12 @@
         <v>2</v>
       </c>
       <c r="F166" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B167" t="s">
         <v>50</v>
@@ -5239,12 +5239,12 @@
         <v>2</v>
       </c>
       <c r="F167" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B168" t="s">
         <v>50</v>
@@ -5259,12 +5259,12 @@
         <v>2</v>
       </c>
       <c r="F168" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B169" t="s">
         <v>50</v>
@@ -5279,12 +5279,12 @@
         <v>2</v>
       </c>
       <c r="F169" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B170" t="s">
         <v>50</v>
@@ -5299,12 +5299,12 @@
         <v>2</v>
       </c>
       <c r="F170" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B171" t="s">
         <v>50</v>
@@ -5319,12 +5319,12 @@
         <v>2</v>
       </c>
       <c r="F171" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B172" t="s">
         <v>50</v>
@@ -5339,12 +5339,12 @@
         <v>2</v>
       </c>
       <c r="F172" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B173" t="s">
         <v>50</v>
@@ -5359,18 +5359,18 @@
         <v>2</v>
       </c>
       <c r="F173" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B174" t="s">
         <v>50</v>
       </c>
       <c r="C174" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D174">
         <v>720</v>
@@ -5379,12 +5379,12 @@
         <v>2</v>
       </c>
       <c r="F174" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B175" t="s">
         <v>50</v>
@@ -5399,18 +5399,18 @@
         <v>2</v>
       </c>
       <c r="F175" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B176" t="s">
         <v>148</v>
       </c>
       <c r="C176" t="s">
-        <v>149</v>
+        <v>494</v>
       </c>
       <c r="D176">
         <v>15000</v>
@@ -5419,18 +5419,18 @@
         <v>2</v>
       </c>
       <c r="F176" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B177" t="s">
         <v>148</v>
       </c>
       <c r="C177" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D177">
         <v>-350</v>
@@ -5439,12 +5439,12 @@
         <v>2</v>
       </c>
       <c r="F177" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B178" t="s">
         <v>47</v>
@@ -5459,12 +5459,12 @@
         <v>2</v>
       </c>
       <c r="F178" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B179" t="s">
         <v>47</v>
@@ -5479,12 +5479,12 @@
         <v>2</v>
       </c>
       <c r="F179" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B180" t="s">
         <v>146</v>
@@ -5499,18 +5499,18 @@
         <v>2</v>
       </c>
       <c r="F180" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B181" t="s">
         <v>146</v>
       </c>
       <c r="C181" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D181">
         <v>-3226</v>
@@ -5519,18 +5519,18 @@
         <v>2</v>
       </c>
       <c r="F181" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B182" t="s">
         <v>146</v>
       </c>
       <c r="C182" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D182">
         <v>-545</v>
@@ -5539,12 +5539,12 @@
         <v>2</v>
       </c>
       <c r="F182" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B183" t="s">
         <v>142</v>
@@ -5559,12 +5559,12 @@
         <v>2</v>
       </c>
       <c r="F183" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B184" t="s">
         <v>142</v>
@@ -5579,12 +5579,12 @@
         <v>2</v>
       </c>
       <c r="F184" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B185" t="s">
         <v>142</v>
@@ -5599,18 +5599,18 @@
         <v>2</v>
       </c>
       <c r="F185" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B186" t="s">
+        <v>252</v>
+      </c>
+      <c r="C186" t="s">
         <v>253</v>
-      </c>
-      <c r="C186" t="s">
-        <v>254</v>
       </c>
       <c r="D186">
         <v>1000</v>
@@ -5619,18 +5619,18 @@
         <v>2</v>
       </c>
       <c r="F186" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B187" t="s">
+        <v>252</v>
+      </c>
+      <c r="C187" t="s">
         <v>253</v>
-      </c>
-      <c r="C187" t="s">
-        <v>254</v>
       </c>
       <c r="D187">
         <v>-1000</v>
@@ -5639,12 +5639,12 @@
         <v>2</v>
       </c>
       <c r="F187" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B188" t="s">
         <v>138</v>
@@ -5659,12 +5659,12 @@
         <v>2</v>
       </c>
       <c r="F188" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B189" t="s">
         <v>138</v>
@@ -5679,12 +5679,12 @@
         <v>2</v>
       </c>
       <c r="F189" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B190" t="s">
         <v>138</v>
@@ -5699,12 +5699,12 @@
         <v>2</v>
       </c>
       <c r="F190" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B191" t="s">
         <v>34</v>
@@ -5719,12 +5719,12 @@
         <v>2</v>
       </c>
       <c r="F191" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B192" t="s">
         <v>34</v>
@@ -5739,12 +5739,12 @@
         <v>2</v>
       </c>
       <c r="F192" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B193" t="s">
         <v>34</v>
@@ -5759,12 +5759,12 @@
         <v>2</v>
       </c>
       <c r="F193" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B194" t="s">
         <v>34</v>
@@ -5779,12 +5779,12 @@
         <v>2</v>
       </c>
       <c r="F194" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B195" t="s">
         <v>34</v>
@@ -5799,12 +5799,12 @@
         <v>2</v>
       </c>
       <c r="F195" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B196" t="s">
         <v>34</v>
@@ -5819,12 +5819,12 @@
         <v>2</v>
       </c>
       <c r="F196" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B197" t="s">
         <v>34</v>
@@ -5839,12 +5839,12 @@
         <v>2</v>
       </c>
       <c r="F197" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B198" t="s">
         <v>34</v>
@@ -5859,12 +5859,12 @@
         <v>2</v>
       </c>
       <c r="F198" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B199" t="s">
         <v>34</v>
@@ -5879,12 +5879,12 @@
         <v>2</v>
       </c>
       <c r="F199" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B200" t="s">
         <v>34</v>
@@ -5899,12 +5899,12 @@
         <v>2</v>
       </c>
       <c r="F200" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B201" t="s">
         <v>34</v>
@@ -5919,12 +5919,12 @@
         <v>2</v>
       </c>
       <c r="F201" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B202" t="s">
         <v>34</v>
@@ -5939,12 +5939,12 @@
         <v>2</v>
       </c>
       <c r="F202" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B203" t="s">
         <v>34</v>
@@ -5959,12 +5959,12 @@
         <v>2</v>
       </c>
       <c r="F203" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B204" t="s">
         <v>34</v>
@@ -5979,18 +5979,18 @@
         <v>2</v>
       </c>
       <c r="F204" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B205" t="s">
         <v>34</v>
       </c>
       <c r="C205" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D205">
         <v>-229</v>
@@ -5999,12 +5999,12 @@
         <v>2</v>
       </c>
       <c r="F205" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B206" t="s">
         <v>28</v>
@@ -6019,12 +6019,12 @@
         <v>2</v>
       </c>
       <c r="F206" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B207" t="s">
         <v>28</v>
@@ -6039,12 +6039,12 @@
         <v>2</v>
       </c>
       <c r="F207" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B208" t="s">
         <v>28</v>
@@ -6059,12 +6059,12 @@
         <v>2</v>
       </c>
       <c r="F208" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B209" t="s">
         <v>28</v>
@@ -6079,12 +6079,12 @@
         <v>2</v>
       </c>
       <c r="F209" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B210" t="s">
         <v>28</v>
@@ -6099,18 +6099,18 @@
         <v>2</v>
       </c>
       <c r="F210" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B211" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C211" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D211">
         <v>1000</v>
@@ -6119,18 +6119,18 @@
         <v>2</v>
       </c>
       <c r="F211" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B212" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C212" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D212">
         <v>-1000</v>
@@ -6139,12 +6139,12 @@
         <v>2</v>
       </c>
       <c r="F212" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B213" t="s">
         <v>21</v>
@@ -6159,12 +6159,12 @@
         <v>2</v>
       </c>
       <c r="F213" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B214" t="s">
         <v>21</v>
@@ -6179,12 +6179,12 @@
         <v>2</v>
       </c>
       <c r="F214" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B215" t="s">
         <v>21</v>
@@ -6199,12 +6199,12 @@
         <v>2</v>
       </c>
       <c r="F215" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B216" t="s">
         <v>21</v>
@@ -6219,12 +6219,12 @@
         <v>2</v>
       </c>
       <c r="F216" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B217" t="s">
         <v>21</v>
@@ -6239,12 +6239,12 @@
         <v>2</v>
       </c>
       <c r="F217" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B218" t="s">
         <v>21</v>
@@ -6259,12 +6259,12 @@
         <v>2</v>
       </c>
       <c r="F218" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B219" t="s">
         <v>126</v>
@@ -6279,12 +6279,12 @@
         <v>2</v>
       </c>
       <c r="F219" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B220" t="s">
         <v>126</v>
@@ -6299,12 +6299,12 @@
         <v>2</v>
       </c>
       <c r="F220" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B221" t="s">
         <v>126</v>
@@ -6319,12 +6319,12 @@
         <v>2</v>
       </c>
       <c r="F221" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B222" t="s">
         <v>126</v>
@@ -6339,12 +6339,12 @@
         <v>2</v>
       </c>
       <c r="F222" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B223" t="s">
         <v>126</v>
@@ -6359,12 +6359,12 @@
         <v>2</v>
       </c>
       <c r="F223" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B224" t="s">
         <v>126</v>
@@ -6379,12 +6379,12 @@
         <v>2</v>
       </c>
       <c r="F224" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B225" t="s">
         <v>126</v>
@@ -6399,18 +6399,18 @@
         <v>2</v>
       </c>
       <c r="F225" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B226" t="s">
         <v>126</v>
       </c>
       <c r="C226" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D226">
         <v>-4500</v>
@@ -6419,12 +6419,12 @@
         <v>2</v>
       </c>
       <c r="F226" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B227" t="s">
         <v>126</v>
@@ -6439,18 +6439,18 @@
         <v>2</v>
       </c>
       <c r="F227" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B228" t="s">
         <v>126</v>
       </c>
       <c r="C228" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D228">
         <v>4000</v>
@@ -6459,18 +6459,18 @@
         <v>2</v>
       </c>
       <c r="F228" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B229" t="s">
         <v>126</v>
       </c>
       <c r="C229" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D229">
         <v>-180</v>
@@ -6479,12 +6479,12 @@
         <v>2</v>
       </c>
       <c r="F229" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B230" t="s">
         <v>126</v>
@@ -6499,12 +6499,12 @@
         <v>2</v>
       </c>
       <c r="F230" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B231" t="s">
         <v>126</v>
@@ -6519,12 +6519,12 @@
         <v>2</v>
       </c>
       <c r="F231" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B232" t="s">
         <v>126</v>
@@ -6539,12 +6539,12 @@
         <v>2</v>
       </c>
       <c r="F232" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B233" t="s">
         <v>126</v>
@@ -6559,12 +6559,12 @@
         <v>2</v>
       </c>
       <c r="F233" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B234" t="s">
         <v>126</v>
@@ -6579,12 +6579,12 @@
         <v>2</v>
       </c>
       <c r="F234" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B235" t="s">
         <v>19</v>
@@ -6599,7 +6599,7 @@
         <v>2</v>
       </c>
       <c r="F235" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some very basic data to other months of 2023
</commit_message>
<xml_diff>
--- a/src/main/resources/transaksjoner.xlsx
+++ b/src/main/resources/transaksjoner.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bjorn\Prosjekter\stacc\SavingApp -backend\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bjorn\Prosjekter\stacc\SavingApp-backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9658BD15-43DF-44C5-A58D-BA129A798BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BD90AD-F89E-4B70-9C14-454E73466EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="527">
   <si>
     <t>06.09.2023</t>
   </si>
@@ -1505,6 +1505,102 @@
   </si>
   <si>
     <t>Nettgiro fra: fdgdfgg Betalt: 25.07.23</t>
+  </si>
+  <si>
+    <t>tx300</t>
+  </si>
+  <si>
+    <t>01.06.2023</t>
+  </si>
+  <si>
+    <t>tx301</t>
+  </si>
+  <si>
+    <t>01.05.2023</t>
+  </si>
+  <si>
+    <t>tx302</t>
+  </si>
+  <si>
+    <t>tx303</t>
+  </si>
+  <si>
+    <t>01.04.2023</t>
+  </si>
+  <si>
+    <t>01.03.2023</t>
+  </si>
+  <si>
+    <t>01.02.2023</t>
+  </si>
+  <si>
+    <t>01.01.2023</t>
+  </si>
+  <si>
+    <t>tx400</t>
+  </si>
+  <si>
+    <t>tx401</t>
+  </si>
+  <si>
+    <t>tx402</t>
+  </si>
+  <si>
+    <t>tx403</t>
+  </si>
+  <si>
+    <t>tx500</t>
+  </si>
+  <si>
+    <t>tx501</t>
+  </si>
+  <si>
+    <t>tx502</t>
+  </si>
+  <si>
+    <t>tx503</t>
+  </si>
+  <si>
+    <t>tx600</t>
+  </si>
+  <si>
+    <t>tx601</t>
+  </si>
+  <si>
+    <t>tx602</t>
+  </si>
+  <si>
+    <t>tx603</t>
+  </si>
+  <si>
+    <t>tx700</t>
+  </si>
+  <si>
+    <t>tx701</t>
+  </si>
+  <si>
+    <t>tx702</t>
+  </si>
+  <si>
+    <t>tx703</t>
+  </si>
+  <si>
+    <t>tx800</t>
+  </si>
+  <si>
+    <t>tx801</t>
+  </si>
+  <si>
+    <t>tx802</t>
+  </si>
+  <si>
+    <t>tx803</t>
+  </si>
+  <si>
+    <t>lånekassen</t>
+  </si>
+  <si>
+    <t>meny</t>
   </si>
 </sst>
 </file>
@@ -1888,10 +1984,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Transaksjoner"/>
-  <dimension ref="A1:F235"/>
+  <dimension ref="A1:F259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="C178" sqref="C178"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="C261" sqref="C261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6602,6 +6698,486 @@
         <v>242</v>
       </c>
     </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>495</v>
+      </c>
+      <c r="B236" t="s">
+        <v>496</v>
+      </c>
+      <c r="C236" t="s">
+        <v>525</v>
+      </c>
+      <c r="D236">
+        <v>15000</v>
+      </c>
+      <c r="E236" t="s">
+        <v>2</v>
+      </c>
+      <c r="F236" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>497</v>
+      </c>
+      <c r="B237" t="s">
+        <v>496</v>
+      </c>
+      <c r="C237" t="s">
+        <v>526</v>
+      </c>
+      <c r="D237">
+        <v>-7500</v>
+      </c>
+      <c r="E237" t="s">
+        <v>2</v>
+      </c>
+      <c r="F237" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>499</v>
+      </c>
+      <c r="B238" t="s">
+        <v>496</v>
+      </c>
+      <c r="C238" t="s">
+        <v>253</v>
+      </c>
+      <c r="D238">
+        <v>1000</v>
+      </c>
+      <c r="E238" t="s">
+        <v>2</v>
+      </c>
+      <c r="F238" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>500</v>
+      </c>
+      <c r="B239" t="s">
+        <v>496</v>
+      </c>
+      <c r="C239" t="s">
+        <v>253</v>
+      </c>
+      <c r="D239">
+        <v>-1000</v>
+      </c>
+      <c r="E239" t="s">
+        <v>2</v>
+      </c>
+      <c r="F239" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>505</v>
+      </c>
+      <c r="B240" t="s">
+        <v>498</v>
+      </c>
+      <c r="C240" t="s">
+        <v>525</v>
+      </c>
+      <c r="D240">
+        <v>15000</v>
+      </c>
+      <c r="E240" t="s">
+        <v>2</v>
+      </c>
+      <c r="F240" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>506</v>
+      </c>
+      <c r="B241" t="s">
+        <v>498</v>
+      </c>
+      <c r="C241" t="s">
+        <v>526</v>
+      </c>
+      <c r="D241">
+        <v>-7500</v>
+      </c>
+      <c r="E241" t="s">
+        <v>2</v>
+      </c>
+      <c r="F241" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>507</v>
+      </c>
+      <c r="B242" t="s">
+        <v>498</v>
+      </c>
+      <c r="C242" t="s">
+        <v>253</v>
+      </c>
+      <c r="D242">
+        <v>1000</v>
+      </c>
+      <c r="E242" t="s">
+        <v>2</v>
+      </c>
+      <c r="F242" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>508</v>
+      </c>
+      <c r="B243" t="s">
+        <v>498</v>
+      </c>
+      <c r="C243" t="s">
+        <v>253</v>
+      </c>
+      <c r="D243">
+        <v>-1000</v>
+      </c>
+      <c r="E243" t="s">
+        <v>2</v>
+      </c>
+      <c r="F243" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>509</v>
+      </c>
+      <c r="B244" t="s">
+        <v>501</v>
+      </c>
+      <c r="C244" t="s">
+        <v>525</v>
+      </c>
+      <c r="D244">
+        <v>15000</v>
+      </c>
+      <c r="E244" t="s">
+        <v>2</v>
+      </c>
+      <c r="F244" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>510</v>
+      </c>
+      <c r="B245" t="s">
+        <v>501</v>
+      </c>
+      <c r="C245" t="s">
+        <v>526</v>
+      </c>
+      <c r="D245">
+        <v>-7500</v>
+      </c>
+      <c r="E245" t="s">
+        <v>2</v>
+      </c>
+      <c r="F245" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>511</v>
+      </c>
+      <c r="B246" t="s">
+        <v>501</v>
+      </c>
+      <c r="C246" t="s">
+        <v>253</v>
+      </c>
+      <c r="D246">
+        <v>1000</v>
+      </c>
+      <c r="E246" t="s">
+        <v>2</v>
+      </c>
+      <c r="F246" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>512</v>
+      </c>
+      <c r="B247" t="s">
+        <v>501</v>
+      </c>
+      <c r="C247" t="s">
+        <v>253</v>
+      </c>
+      <c r="D247">
+        <v>-1000</v>
+      </c>
+      <c r="E247" t="s">
+        <v>2</v>
+      </c>
+      <c r="F247" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>513</v>
+      </c>
+      <c r="B248" t="s">
+        <v>502</v>
+      </c>
+      <c r="C248" t="s">
+        <v>525</v>
+      </c>
+      <c r="D248">
+        <v>15000</v>
+      </c>
+      <c r="E248" t="s">
+        <v>2</v>
+      </c>
+      <c r="F248" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>514</v>
+      </c>
+      <c r="B249" t="s">
+        <v>502</v>
+      </c>
+      <c r="C249" t="s">
+        <v>526</v>
+      </c>
+      <c r="D249">
+        <v>-7500</v>
+      </c>
+      <c r="E249" t="s">
+        <v>2</v>
+      </c>
+      <c r="F249" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>515</v>
+      </c>
+      <c r="B250" t="s">
+        <v>502</v>
+      </c>
+      <c r="C250" t="s">
+        <v>253</v>
+      </c>
+      <c r="D250">
+        <v>1000</v>
+      </c>
+      <c r="E250" t="s">
+        <v>2</v>
+      </c>
+      <c r="F250" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>516</v>
+      </c>
+      <c r="B251" t="s">
+        <v>502</v>
+      </c>
+      <c r="C251" t="s">
+        <v>253</v>
+      </c>
+      <c r="D251">
+        <v>-1000</v>
+      </c>
+      <c r="E251" t="s">
+        <v>2</v>
+      </c>
+      <c r="F251" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>517</v>
+      </c>
+      <c r="B252" t="s">
+        <v>503</v>
+      </c>
+      <c r="C252" t="s">
+        <v>525</v>
+      </c>
+      <c r="D252">
+        <v>15000</v>
+      </c>
+      <c r="E252" t="s">
+        <v>2</v>
+      </c>
+      <c r="F252" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>518</v>
+      </c>
+      <c r="B253" t="s">
+        <v>503</v>
+      </c>
+      <c r="C253" t="s">
+        <v>526</v>
+      </c>
+      <c r="D253">
+        <v>-7500</v>
+      </c>
+      <c r="E253" t="s">
+        <v>2</v>
+      </c>
+      <c r="F253" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>519</v>
+      </c>
+      <c r="B254" t="s">
+        <v>503</v>
+      </c>
+      <c r="C254" t="s">
+        <v>253</v>
+      </c>
+      <c r="D254">
+        <v>1000</v>
+      </c>
+      <c r="E254" t="s">
+        <v>2</v>
+      </c>
+      <c r="F254" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>520</v>
+      </c>
+      <c r="B255" t="s">
+        <v>503</v>
+      </c>
+      <c r="C255" t="s">
+        <v>253</v>
+      </c>
+      <c r="D255">
+        <v>-1000</v>
+      </c>
+      <c r="E255" t="s">
+        <v>2</v>
+      </c>
+      <c r="F255" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>521</v>
+      </c>
+      <c r="B256" t="s">
+        <v>504</v>
+      </c>
+      <c r="C256" t="s">
+        <v>525</v>
+      </c>
+      <c r="D256">
+        <v>15000</v>
+      </c>
+      <c r="E256" t="s">
+        <v>2</v>
+      </c>
+      <c r="F256" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>522</v>
+      </c>
+      <c r="B257" t="s">
+        <v>504</v>
+      </c>
+      <c r="C257" t="s">
+        <v>526</v>
+      </c>
+      <c r="D257">
+        <v>-7500</v>
+      </c>
+      <c r="E257" t="s">
+        <v>2</v>
+      </c>
+      <c r="F257" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>523</v>
+      </c>
+      <c r="B258" t="s">
+        <v>504</v>
+      </c>
+      <c r="C258" t="s">
+        <v>253</v>
+      </c>
+      <c r="D258">
+        <v>1000</v>
+      </c>
+      <c r="E258" t="s">
+        <v>2</v>
+      </c>
+      <c r="F258" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>524</v>
+      </c>
+      <c r="B259" t="s">
+        <v>504</v>
+      </c>
+      <c r="C259" t="s">
+        <v>253</v>
+      </c>
+      <c r="D259">
+        <v>-1000</v>
+      </c>
+      <c r="E259" t="s">
+        <v>2</v>
+      </c>
+      <c r="F259" t="s">
+        <v>242</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F235">
     <sortCondition ref="B2:B235"/>

</xml_diff>